<commit_message>
adding daily positive rates and mobility index charts to the mix; minor edits
</commit_message>
<xml_diff>
--- a/data/beds-vent.xlsx
+++ b/data/beds-vent.xlsx
@@ -385,7 +385,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1484</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="3">
@@ -395,7 +395,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3264</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +405,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>570</v>
+        <v>514</v>
       </c>
     </row>
     <row r="5">
@@ -415,7 +415,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1277</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="6">
@@ -425,7 +425,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1417</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="7">
@@ -435,7 +435,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3189</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="8">
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9">
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>379</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2548</v>
+        <v>2463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>